<commit_message>
Now using spyder for increased functionality
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livewarwickac-my.sharepoint.com/personal/u1606521_live_warwick_ac_uk/Documents/Year 3/Dissertation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\callu\OneDrive for Business\Year 3\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFCEAFF3-7D22-49B9-9A62-692893E1B0C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FFCEAFF3-7D22-49B9-9A62-692893E1B0C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{52393492-C070-4373-B982-811353E76980}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1112,9 +1112,6 @@
     <t>Drop</t>
   </si>
   <si>
-    <t>Pheonix</t>
-  </si>
-  <si>
     <t>Track</t>
   </si>
   <si>
@@ -3384,6 +3381,9 @@
   </si>
   <si>
     <t>Attic</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
   </si>
 </sst>
 </file>
@@ -3760,7 +3760,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3910,7 +3910,7 @@
         <v>360</v>
       </c>
       <c r="N3" t="s">
-        <v>361</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3951,10 +3951,10 @@
         <v>304</v>
       </c>
       <c r="M4" t="s">
+        <v>361</v>
+      </c>
+      <c r="N4" t="s">
         <v>362</v>
-      </c>
-      <c r="N4" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -3995,10 +3995,10 @@
         <v>306</v>
       </c>
       <c r="M5" t="s">
+        <v>363</v>
+      </c>
+      <c r="N5" t="s">
         <v>364</v>
-      </c>
-      <c r="N5" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4039,10 +4039,10 @@
         <v>308</v>
       </c>
       <c r="M6" t="s">
+        <v>365</v>
+      </c>
+      <c r="N6" t="s">
         <v>366</v>
-      </c>
-      <c r="N6" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4083,10 +4083,10 @@
         <v>310</v>
       </c>
       <c r="M7" t="s">
+        <v>367</v>
+      </c>
+      <c r="N7" t="s">
         <v>368</v>
-      </c>
-      <c r="N7" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4127,10 +4127,10 @@
         <v>312</v>
       </c>
       <c r="M8" t="s">
+        <v>369</v>
+      </c>
+      <c r="N8" t="s">
         <v>370</v>
-      </c>
-      <c r="N8" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4171,10 +4171,10 @@
         <v>314</v>
       </c>
       <c r="M9" t="s">
+        <v>371</v>
+      </c>
+      <c r="N9" t="s">
         <v>372</v>
-      </c>
-      <c r="N9" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4215,10 +4215,10 @@
         <v>316</v>
       </c>
       <c r="M10" t="s">
+        <v>373</v>
+      </c>
+      <c r="N10" t="s">
         <v>374</v>
-      </c>
-      <c r="N10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4259,10 +4259,10 @@
         <v>318</v>
       </c>
       <c r="M11" t="s">
+        <v>375</v>
+      </c>
+      <c r="N11" t="s">
         <v>376</v>
-      </c>
-      <c r="N11" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -4279,7 +4279,7 @@
         <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F12" t="s">
         <v>140</v>
@@ -4303,10 +4303,10 @@
         <v>320</v>
       </c>
       <c r="M12" t="s">
+        <v>377</v>
+      </c>
+      <c r="N12" t="s">
         <v>378</v>
-      </c>
-      <c r="N12" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -4347,10 +4347,10 @@
         <v>322</v>
       </c>
       <c r="M13" t="s">
+        <v>379</v>
+      </c>
+      <c r="N13" t="s">
         <v>380</v>
-      </c>
-      <c r="N13" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4391,10 +4391,10 @@
         <v>324</v>
       </c>
       <c r="M14" t="s">
+        <v>381</v>
+      </c>
+      <c r="N14" t="s">
         <v>382</v>
-      </c>
-      <c r="N14" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4435,10 +4435,10 @@
         <v>326</v>
       </c>
       <c r="M15" t="s">
+        <v>383</v>
+      </c>
+      <c r="N15" t="s">
         <v>384</v>
-      </c>
-      <c r="N15" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -4479,10 +4479,10 @@
         <v>328</v>
       </c>
       <c r="M16" t="s">
+        <v>385</v>
+      </c>
+      <c r="N16" t="s">
         <v>386</v>
-      </c>
-      <c r="N16" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -4523,10 +4523,10 @@
         <v>330</v>
       </c>
       <c r="M17" t="s">
+        <v>387</v>
+      </c>
+      <c r="N17" t="s">
         <v>388</v>
-      </c>
-      <c r="N17" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -4567,10 +4567,10 @@
         <v>332</v>
       </c>
       <c r="M18" t="s">
+        <v>389</v>
+      </c>
+      <c r="N18" t="s">
         <v>390</v>
-      </c>
-      <c r="N18" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -4611,10 +4611,10 @@
         <v>334</v>
       </c>
       <c r="M19" t="s">
+        <v>391</v>
+      </c>
+      <c r="N19" t="s">
         <v>392</v>
-      </c>
-      <c r="N19" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4655,10 +4655,10 @@
         <v>336</v>
       </c>
       <c r="M20" t="s">
+        <v>393</v>
+      </c>
+      <c r="N20" t="s">
         <v>394</v>
-      </c>
-      <c r="N20" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
         <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E23" t="s">
         <v>161</v>
@@ -4810,7 +4810,7 @@
         <v>343</v>
       </c>
       <c r="L24" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -5011,7 +5011,7 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D30" t="s">
         <v>117</v>
@@ -5072,84 +5072,84 @@
         <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E1" t="s">
         <v>450</v>
-      </c>
-      <c r="E1" t="s">
-        <v>451</v>
       </c>
       <c r="G1" t="s">
         <v>206</v>
       </c>
       <c r="H1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J1" t="s">
+        <v>557</v>
+      </c>
+      <c r="K1" t="s">
         <v>558</v>
       </c>
-      <c r="K1" t="s">
-        <v>559</v>
-      </c>
       <c r="M1" t="s">
+        <v>611</v>
+      </c>
+      <c r="N1" t="s">
         <v>612</v>
       </c>
-      <c r="N1" t="s">
-        <v>613</v>
-      </c>
       <c r="P1" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q1" t="s">
         <v>666</v>
       </c>
-      <c r="Q1" t="s">
-        <v>667</v>
-      </c>
       <c r="S1" t="s">
+        <v>716</v>
+      </c>
+      <c r="T1" t="s">
         <v>717</v>
-      </c>
-      <c r="T1" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" t="s">
         <v>398</v>
       </c>
-      <c r="B2" t="s">
-        <v>399</v>
-      </c>
       <c r="D2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E2" t="s">
         <v>452</v>
       </c>
-      <c r="E2" t="s">
-        <v>453</v>
-      </c>
       <c r="G2" t="s">
+        <v>507</v>
+      </c>
+      <c r="H2" t="s">
         <v>508</v>
       </c>
-      <c r="H2" t="s">
-        <v>509</v>
-      </c>
       <c r="J2" t="s">
+        <v>559</v>
+      </c>
+      <c r="K2" t="s">
         <v>560</v>
       </c>
-      <c r="K2" t="s">
-        <v>561</v>
-      </c>
       <c r="M2" t="s">
+        <v>613</v>
+      </c>
+      <c r="N2" t="s">
         <v>614</v>
       </c>
-      <c r="N2" t="s">
-        <v>615</v>
-      </c>
       <c r="P2" t="s">
+        <v>667</v>
+      </c>
+      <c r="Q2" t="s">
         <v>668</v>
       </c>
-      <c r="Q2" t="s">
-        <v>669</v>
-      </c>
       <c r="S2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="T2" t="s">
         <v>23</v>
@@ -5157,219 +5157,219 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" t="s">
         <v>400</v>
       </c>
-      <c r="B3" t="s">
-        <v>401</v>
-      </c>
       <c r="D3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E3" t="s">
         <v>454</v>
       </c>
-      <c r="E3" t="s">
-        <v>455</v>
-      </c>
       <c r="G3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H3" t="s">
         <v>195</v>
       </c>
       <c r="J3" t="s">
+        <v>561</v>
+      </c>
+      <c r="K3" t="s">
         <v>562</v>
       </c>
-      <c r="K3" t="s">
-        <v>563</v>
-      </c>
       <c r="M3" t="s">
+        <v>615</v>
+      </c>
+      <c r="N3" t="s">
         <v>616</v>
       </c>
-      <c r="N3" t="s">
-        <v>617</v>
-      </c>
       <c r="P3" t="s">
+        <v>669</v>
+      </c>
+      <c r="Q3" t="s">
         <v>670</v>
       </c>
-      <c r="Q3" t="s">
-        <v>671</v>
-      </c>
       <c r="S3" t="s">
+        <v>719</v>
+      </c>
+      <c r="T3" t="s">
         <v>720</v>
-      </c>
-      <c r="T3" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D4" t="s">
+        <v>455</v>
+      </c>
+      <c r="E4" t="s">
         <v>456</v>
       </c>
-      <c r="E4" t="s">
-        <v>457</v>
-      </c>
       <c r="G4" t="s">
+        <v>510</v>
+      </c>
+      <c r="H4" t="s">
         <v>511</v>
       </c>
-      <c r="H4" t="s">
-        <v>512</v>
-      </c>
       <c r="J4" t="s">
+        <v>563</v>
+      </c>
+      <c r="K4" t="s">
         <v>564</v>
       </c>
-      <c r="K4" t="s">
-        <v>565</v>
-      </c>
       <c r="M4" t="s">
+        <v>617</v>
+      </c>
+      <c r="N4" t="s">
         <v>618</v>
       </c>
-      <c r="N4" t="s">
-        <v>619</v>
-      </c>
       <c r="P4" t="s">
+        <v>671</v>
+      </c>
+      <c r="Q4" t="s">
         <v>672</v>
       </c>
-      <c r="Q4" t="s">
-        <v>673</v>
-      </c>
       <c r="S4" t="s">
+        <v>721</v>
+      </c>
+      <c r="T4" t="s">
         <v>722</v>
-      </c>
-      <c r="T4" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B5" t="s">
         <v>403</v>
       </c>
-      <c r="B5" t="s">
-        <v>404</v>
-      </c>
       <c r="D5" t="s">
+        <v>457</v>
+      </c>
+      <c r="E5" t="s">
         <v>458</v>
       </c>
-      <c r="E5" t="s">
-        <v>459</v>
-      </c>
       <c r="G5" t="s">
+        <v>512</v>
+      </c>
+      <c r="H5" t="s">
         <v>513</v>
-      </c>
-      <c r="H5" t="s">
-        <v>514</v>
       </c>
       <c r="J5" t="s">
         <v>281</v>
       </c>
       <c r="K5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="M5" t="s">
+        <v>619</v>
+      </c>
+      <c r="N5" t="s">
         <v>620</v>
       </c>
-      <c r="N5" t="s">
-        <v>621</v>
-      </c>
       <c r="P5" t="s">
+        <v>673</v>
+      </c>
+      <c r="Q5" t="s">
         <v>674</v>
       </c>
-      <c r="Q5" t="s">
-        <v>675</v>
-      </c>
       <c r="S5" t="s">
+        <v>723</v>
+      </c>
+      <c r="T5" t="s">
         <v>724</v>
-      </c>
-      <c r="T5" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>404</v>
+      </c>
+      <c r="B6" t="s">
         <v>405</v>
       </c>
-      <c r="B6" t="s">
-        <v>406</v>
-      </c>
       <c r="D6" t="s">
+        <v>459</v>
+      </c>
+      <c r="E6" t="s">
         <v>460</v>
       </c>
-      <c r="E6" t="s">
-        <v>461</v>
-      </c>
       <c r="G6" t="s">
+        <v>514</v>
+      </c>
+      <c r="H6" t="s">
         <v>515</v>
       </c>
-      <c r="H6" t="s">
-        <v>516</v>
-      </c>
       <c r="J6" t="s">
+        <v>566</v>
+      </c>
+      <c r="K6" t="s">
         <v>567</v>
       </c>
-      <c r="K6" t="s">
-        <v>568</v>
-      </c>
       <c r="M6" t="s">
+        <v>621</v>
+      </c>
+      <c r="N6" t="s">
         <v>622</v>
       </c>
-      <c r="N6" t="s">
-        <v>623</v>
-      </c>
       <c r="P6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="S6" t="s">
+        <v>725</v>
+      </c>
+      <c r="T6" t="s">
         <v>726</v>
-      </c>
-      <c r="T6" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>406</v>
+      </c>
+      <c r="B7" t="s">
         <v>407</v>
       </c>
-      <c r="B7" t="s">
-        <v>408</v>
-      </c>
       <c r="D7" t="s">
+        <v>461</v>
+      </c>
+      <c r="E7" t="s">
         <v>462</v>
       </c>
-      <c r="E7" t="s">
-        <v>463</v>
-      </c>
       <c r="G7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H7" t="s">
         <v>161</v>
       </c>
       <c r="J7" t="s">
+        <v>568</v>
+      </c>
+      <c r="K7" t="s">
         <v>569</v>
       </c>
-      <c r="K7" t="s">
-        <v>570</v>
-      </c>
       <c r="M7" t="s">
+        <v>623</v>
+      </c>
+      <c r="N7" t="s">
         <v>624</v>
       </c>
-      <c r="N7" t="s">
-        <v>625</v>
-      </c>
       <c r="P7" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q7" t="s">
         <v>677</v>
       </c>
-      <c r="Q7" t="s">
-        <v>678</v>
-      </c>
       <c r="S7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="T7" t="s">
         <v>44</v>
@@ -5377,90 +5377,90 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B8" t="s">
         <v>409</v>
       </c>
-      <c r="B8" t="s">
-        <v>410</v>
-      </c>
       <c r="D8" t="s">
+        <v>463</v>
+      </c>
+      <c r="E8" t="s">
         <v>464</v>
       </c>
-      <c r="E8" t="s">
-        <v>465</v>
-      </c>
       <c r="G8" t="s">
+        <v>517</v>
+      </c>
+      <c r="H8" t="s">
         <v>518</v>
       </c>
-      <c r="H8" t="s">
-        <v>519</v>
-      </c>
       <c r="J8" t="s">
+        <v>570</v>
+      </c>
+      <c r="K8" t="s">
         <v>571</v>
       </c>
-      <c r="K8" t="s">
-        <v>572</v>
-      </c>
       <c r="M8" t="s">
+        <v>625</v>
+      </c>
+      <c r="N8" t="s">
         <v>626</v>
-      </c>
-      <c r="N8" t="s">
-        <v>627</v>
       </c>
       <c r="P8" t="s">
         <v>252</v>
       </c>
       <c r="Q8" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="S8" t="s">
+        <v>728</v>
+      </c>
+      <c r="T8" t="s">
         <v>729</v>
-      </c>
-      <c r="T8" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" t="s">
         <v>411</v>
       </c>
-      <c r="B9" t="s">
-        <v>412</v>
-      </c>
       <c r="D9" t="s">
+        <v>465</v>
+      </c>
+      <c r="E9" t="s">
         <v>466</v>
-      </c>
-      <c r="E9" t="s">
-        <v>467</v>
       </c>
       <c r="G9" t="s">
         <v>223</v>
       </c>
       <c r="H9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J9" t="s">
+        <v>572</v>
+      </c>
+      <c r="K9" t="s">
         <v>573</v>
       </c>
-      <c r="K9" t="s">
-        <v>574</v>
-      </c>
       <c r="M9" t="s">
+        <v>627</v>
+      </c>
+      <c r="N9" t="s">
         <v>628</v>
       </c>
-      <c r="N9" t="s">
-        <v>629</v>
-      </c>
       <c r="P9" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q9" t="s">
         <v>680</v>
       </c>
-      <c r="Q9" t="s">
-        <v>681</v>
-      </c>
       <c r="S9" t="s">
+        <v>730</v>
+      </c>
+      <c r="T9" t="s">
         <v>731</v>
-      </c>
-      <c r="T9" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -5468,40 +5468,40 @@
         <v>210</v>
       </c>
       <c r="B10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E10" t="s">
         <v>468</v>
       </c>
-      <c r="E10" t="s">
-        <v>469</v>
-      </c>
       <c r="G10" t="s">
+        <v>520</v>
+      </c>
+      <c r="H10" t="s">
         <v>521</v>
       </c>
-      <c r="H10" t="s">
-        <v>522</v>
-      </c>
       <c r="J10" t="s">
+        <v>574</v>
+      </c>
+      <c r="K10" t="s">
         <v>575</v>
       </c>
-      <c r="K10" t="s">
-        <v>576</v>
-      </c>
       <c r="M10" t="s">
+        <v>629</v>
+      </c>
+      <c r="N10" t="s">
         <v>630</v>
       </c>
-      <c r="N10" t="s">
-        <v>631</v>
-      </c>
       <c r="P10" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q10" t="s">
         <v>682</v>
       </c>
-      <c r="Q10" t="s">
-        <v>683</v>
-      </c>
       <c r="S10" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="T10" t="s">
         <v>98</v>
@@ -5509,46 +5509,46 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>413</v>
+      </c>
+      <c r="B11" t="s">
         <v>414</v>
       </c>
-      <c r="B11" t="s">
-        <v>415</v>
-      </c>
       <c r="D11" t="s">
+        <v>469</v>
+      </c>
+      <c r="E11" t="s">
         <v>470</v>
       </c>
-      <c r="E11" t="s">
-        <v>471</v>
-      </c>
       <c r="G11" t="s">
+        <v>522</v>
+      </c>
+      <c r="H11" t="s">
         <v>523</v>
       </c>
-      <c r="H11" t="s">
-        <v>524</v>
-      </c>
       <c r="J11" t="s">
+        <v>576</v>
+      </c>
+      <c r="K11" t="s">
         <v>577</v>
       </c>
-      <c r="K11" t="s">
-        <v>578</v>
-      </c>
       <c r="M11" t="s">
+        <v>631</v>
+      </c>
+      <c r="N11" t="s">
         <v>632</v>
       </c>
-      <c r="N11" t="s">
-        <v>633</v>
-      </c>
       <c r="P11" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q11" t="s">
         <v>684</v>
       </c>
-      <c r="Q11" t="s">
-        <v>685</v>
-      </c>
       <c r="S11" t="s">
+        <v>733</v>
+      </c>
+      <c r="T11" t="s">
         <v>734</v>
-      </c>
-      <c r="T11" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -5556,40 +5556,40 @@
         <v>203</v>
       </c>
       <c r="B12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D12" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E12" t="s">
         <v>254</v>
       </c>
       <c r="G12" t="s">
+        <v>524</v>
+      </c>
+      <c r="H12" t="s">
         <v>525</v>
       </c>
-      <c r="H12" t="s">
-        <v>526</v>
-      </c>
       <c r="J12" t="s">
+        <v>578</v>
+      </c>
+      <c r="K12" t="s">
         <v>579</v>
-      </c>
-      <c r="K12" t="s">
-        <v>580</v>
       </c>
       <c r="M12" t="s">
         <v>344</v>
       </c>
       <c r="N12" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="P12" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="Q12" t="s">
         <v>155</v>
       </c>
       <c r="S12" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="T12" t="s">
         <v>33</v>
@@ -5597,13 +5597,13 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>416</v>
+      </c>
+      <c r="B13" t="s">
         <v>417</v>
       </c>
-      <c r="B13" t="s">
-        <v>418</v>
-      </c>
       <c r="D13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E13" t="s">
         <v>205</v>
@@ -5612,101 +5612,101 @@
         <v>176</v>
       </c>
       <c r="H13" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J13" t="s">
         <v>316</v>
       </c>
       <c r="K13" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M13" t="s">
+        <v>634</v>
+      </c>
+      <c r="N13" t="s">
         <v>635</v>
       </c>
-      <c r="N13" t="s">
-        <v>636</v>
-      </c>
       <c r="P13" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q13" t="s">
         <v>687</v>
       </c>
-      <c r="Q13" t="s">
-        <v>688</v>
-      </c>
       <c r="S13" t="s">
+        <v>736</v>
+      </c>
+      <c r="T13" t="s">
         <v>737</v>
-      </c>
-      <c r="T13" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>418</v>
+      </c>
+      <c r="B14" t="s">
         <v>419</v>
       </c>
-      <c r="B14" t="s">
-        <v>420</v>
-      </c>
       <c r="D14" t="s">
+        <v>473</v>
+      </c>
+      <c r="E14" t="s">
         <v>474</v>
       </c>
-      <c r="E14" t="s">
-        <v>475</v>
-      </c>
       <c r="G14" t="s">
+        <v>527</v>
+      </c>
+      <c r="H14" t="s">
         <v>528</v>
       </c>
-      <c r="H14" t="s">
-        <v>529</v>
-      </c>
       <c r="J14" t="s">
+        <v>581</v>
+      </c>
+      <c r="K14" t="s">
         <v>582</v>
       </c>
-      <c r="K14" t="s">
-        <v>583</v>
-      </c>
       <c r="M14" t="s">
+        <v>636</v>
+      </c>
+      <c r="N14" t="s">
         <v>637</v>
       </c>
-      <c r="N14" t="s">
-        <v>638</v>
-      </c>
       <c r="P14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="Q14" t="s">
         <v>235</v>
       </c>
       <c r="S14" t="s">
+        <v>738</v>
+      </c>
+      <c r="T14" t="s">
         <v>739</v>
-      </c>
-      <c r="T14" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>420</v>
+      </c>
+      <c r="B15" t="s">
         <v>421</v>
       </c>
-      <c r="B15" t="s">
-        <v>422</v>
-      </c>
       <c r="D15" t="s">
+        <v>475</v>
+      </c>
+      <c r="E15" t="s">
         <v>476</v>
-      </c>
-      <c r="E15" t="s">
-        <v>477</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J15" t="s">
+        <v>583</v>
+      </c>
+      <c r="K15" t="s">
         <v>584</v>
-      </c>
-      <c r="K15" t="s">
-        <v>585</v>
       </c>
       <c r="M15" t="s">
         <v>290</v>
@@ -5718,13 +5718,13 @@
         <v>319</v>
       </c>
       <c r="Q15" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S15" t="s">
+        <v>740</v>
+      </c>
+      <c r="T15" t="s">
         <v>741</v>
-      </c>
-      <c r="T15" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -5732,37 +5732,37 @@
         <v>183</v>
       </c>
       <c r="B16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D16" t="s">
+        <v>477</v>
+      </c>
+      <c r="E16" t="s">
         <v>478</v>
       </c>
-      <c r="E16" t="s">
-        <v>479</v>
-      </c>
       <c r="G16" t="s">
+        <v>530</v>
+      </c>
+      <c r="H16" t="s">
         <v>531</v>
       </c>
-      <c r="H16" t="s">
-        <v>532</v>
-      </c>
       <c r="J16" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="K16" t="s">
         <v>327</v>
       </c>
       <c r="M16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="P16" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q16" t="s">
         <v>691</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>692</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -5772,114 +5772,114 @@
         <v>270</v>
       </c>
       <c r="B17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D17" t="s">
+        <v>479</v>
+      </c>
+      <c r="E17" t="s">
         <v>480</v>
       </c>
-      <c r="E17" t="s">
-        <v>481</v>
-      </c>
       <c r="G17" t="s">
+        <v>532</v>
+      </c>
+      <c r="H17" t="s">
         <v>533</v>
       </c>
-      <c r="H17" t="s">
-        <v>534</v>
-      </c>
       <c r="J17" t="s">
+        <v>586</v>
+      </c>
+      <c r="K17" t="s">
         <v>587</v>
       </c>
-      <c r="K17" t="s">
-        <v>588</v>
-      </c>
       <c r="M17" t="s">
+        <v>639</v>
+      </c>
+      <c r="N17" t="s">
         <v>640</v>
       </c>
-      <c r="N17" t="s">
-        <v>641</v>
-      </c>
       <c r="P17" t="s">
+        <v>692</v>
+      </c>
+      <c r="Q17" t="s">
         <v>693</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>694</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>424</v>
+      </c>
+      <c r="B18" t="s">
         <v>425</v>
       </c>
-      <c r="B18" t="s">
-        <v>426</v>
-      </c>
       <c r="D18" t="s">
+        <v>481</v>
+      </c>
+      <c r="E18" t="s">
         <v>482</v>
       </c>
-      <c r="E18" t="s">
-        <v>483</v>
-      </c>
       <c r="G18" t="s">
+        <v>534</v>
+      </c>
+      <c r="H18" t="s">
         <v>535</v>
       </c>
-      <c r="H18" t="s">
-        <v>536</v>
-      </c>
       <c r="J18" t="s">
+        <v>588</v>
+      </c>
+      <c r="K18" t="s">
         <v>589</v>
       </c>
-      <c r="K18" t="s">
-        <v>590</v>
-      </c>
       <c r="M18" t="s">
+        <v>742</v>
+      </c>
+      <c r="N18" t="s">
         <v>743</v>
       </c>
-      <c r="N18" t="s">
-        <v>744</v>
-      </c>
       <c r="P18" t="s">
+        <v>694</v>
+      </c>
+      <c r="Q18" t="s">
         <v>695</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>696</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>426</v>
+      </c>
+      <c r="B19" t="s">
         <v>427</v>
       </c>
-      <c r="B19" t="s">
-        <v>428</v>
-      </c>
       <c r="D19" t="s">
+        <v>483</v>
+      </c>
+      <c r="E19" t="s">
         <v>484</v>
       </c>
-      <c r="E19" t="s">
-        <v>485</v>
-      </c>
       <c r="G19" t="s">
+        <v>536</v>
+      </c>
+      <c r="H19" t="s">
         <v>537</v>
       </c>
-      <c r="H19" t="s">
-        <v>538</v>
-      </c>
       <c r="J19" t="s">
+        <v>590</v>
+      </c>
+      <c r="K19" t="s">
         <v>591</v>
       </c>
-      <c r="K19" t="s">
-        <v>592</v>
-      </c>
       <c r="M19" t="s">
+        <v>641</v>
+      </c>
+      <c r="N19" t="s">
         <v>642</v>
       </c>
-      <c r="N19" t="s">
-        <v>643</v>
-      </c>
       <c r="P19" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q19" t="s">
         <v>14</v>
@@ -5889,115 +5889,115 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>428</v>
+      </c>
+      <c r="B20" t="s">
         <v>429</v>
       </c>
-      <c r="B20" t="s">
-        <v>430</v>
-      </c>
       <c r="D20" t="s">
+        <v>485</v>
+      </c>
+      <c r="E20" t="s">
         <v>486</v>
       </c>
-      <c r="E20" t="s">
-        <v>487</v>
-      </c>
       <c r="G20" t="s">
+        <v>538</v>
+      </c>
+      <c r="H20" t="s">
         <v>539</v>
       </c>
-      <c r="H20" t="s">
-        <v>540</v>
-      </c>
       <c r="J20" t="s">
+        <v>592</v>
+      </c>
+      <c r="K20" t="s">
         <v>593</v>
       </c>
-      <c r="K20" t="s">
-        <v>594</v>
-      </c>
       <c r="M20" t="s">
+        <v>643</v>
+      </c>
+      <c r="N20" t="s">
         <v>644</v>
       </c>
-      <c r="N20" t="s">
-        <v>645</v>
-      </c>
       <c r="P20" t="s">
+        <v>697</v>
+      </c>
+      <c r="Q20" t="s">
         <v>698</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>699</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>430</v>
+      </c>
+      <c r="B21" t="s">
         <v>431</v>
       </c>
-      <c r="B21" t="s">
-        <v>432</v>
-      </c>
       <c r="D21" t="s">
+        <v>487</v>
+      </c>
+      <c r="E21" t="s">
         <v>488</v>
       </c>
-      <c r="E21" t="s">
-        <v>489</v>
-      </c>
       <c r="G21" t="s">
+        <v>540</v>
+      </c>
+      <c r="H21" t="s">
         <v>541</v>
       </c>
-      <c r="H21" t="s">
-        <v>542</v>
-      </c>
       <c r="J21" t="s">
+        <v>594</v>
+      </c>
+      <c r="K21" t="s">
         <v>595</v>
       </c>
-      <c r="K21" t="s">
-        <v>596</v>
-      </c>
       <c r="M21" t="s">
+        <v>645</v>
+      </c>
+      <c r="N21" t="s">
         <v>646</v>
       </c>
-      <c r="N21" t="s">
-        <v>647</v>
-      </c>
       <c r="P21" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q21" t="s">
         <v>700</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>432</v>
+      </c>
+      <c r="B22" t="s">
         <v>433</v>
       </c>
-      <c r="B22" t="s">
-        <v>434</v>
-      </c>
       <c r="D22" t="s">
+        <v>489</v>
+      </c>
+      <c r="E22" t="s">
         <v>490</v>
       </c>
-      <c r="E22" t="s">
-        <v>491</v>
-      </c>
       <c r="G22" t="s">
+        <v>542</v>
+      </c>
+      <c r="H22" t="s">
         <v>543</v>
       </c>
-      <c r="H22" t="s">
-        <v>544</v>
-      </c>
       <c r="J22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="K22" t="s">
         <v>347</v>
       </c>
       <c r="M22" t="s">
+        <v>647</v>
+      </c>
+      <c r="N22" t="s">
         <v>648</v>
       </c>
-      <c r="N22" t="s">
-        <v>649</v>
-      </c>
       <c r="P22" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="Q22" t="s">
         <v>213</v>
@@ -6005,230 +6005,230 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>434</v>
+      </c>
+      <c r="B23" t="s">
         <v>435</v>
       </c>
-      <c r="B23" t="s">
-        <v>436</v>
-      </c>
       <c r="D23" t="s">
+        <v>491</v>
+      </c>
+      <c r="E23" t="s">
         <v>492</v>
       </c>
-      <c r="E23" t="s">
-        <v>493</v>
-      </c>
       <c r="G23" t="s">
+        <v>544</v>
+      </c>
+      <c r="H23" t="s">
         <v>545</v>
-      </c>
-      <c r="H23" t="s">
-        <v>546</v>
       </c>
       <c r="J23" t="s">
         <v>146</v>
       </c>
       <c r="K23" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M23" t="s">
+        <v>649</v>
+      </c>
+      <c r="N23" t="s">
         <v>650</v>
-      </c>
-      <c r="N23" t="s">
-        <v>651</v>
       </c>
       <c r="P23" t="s">
         <v>306</v>
       </c>
       <c r="Q23" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>436</v>
+      </c>
+      <c r="B24" t="s">
         <v>437</v>
       </c>
-      <c r="B24" t="s">
-        <v>438</v>
-      </c>
       <c r="D24" t="s">
+        <v>493</v>
+      </c>
+      <c r="E24" t="s">
         <v>494</v>
       </c>
-      <c r="E24" t="s">
-        <v>495</v>
-      </c>
       <c r="G24" t="s">
+        <v>546</v>
+      </c>
+      <c r="H24" t="s">
         <v>547</v>
       </c>
-      <c r="H24" t="s">
-        <v>548</v>
-      </c>
       <c r="J24" t="s">
+        <v>598</v>
+      </c>
+      <c r="K24" t="s">
         <v>599</v>
       </c>
-      <c r="K24" t="s">
-        <v>600</v>
-      </c>
       <c r="M24" t="s">
+        <v>651</v>
+      </c>
+      <c r="N24" t="s">
         <v>652</v>
       </c>
-      <c r="N24" t="s">
-        <v>653</v>
-      </c>
       <c r="P24" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q24" t="s">
         <v>704</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>438</v>
+      </c>
+      <c r="B25" t="s">
         <v>439</v>
       </c>
-      <c r="B25" t="s">
-        <v>440</v>
-      </c>
       <c r="D25" t="s">
+        <v>495</v>
+      </c>
+      <c r="E25" t="s">
         <v>496</v>
       </c>
-      <c r="E25" t="s">
-        <v>497</v>
-      </c>
       <c r="G25" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H25" t="s">
         <v>50</v>
       </c>
       <c r="J25" t="s">
+        <v>600</v>
+      </c>
+      <c r="K25" t="s">
         <v>601</v>
       </c>
-      <c r="K25" t="s">
-        <v>602</v>
-      </c>
       <c r="M25" t="s">
+        <v>653</v>
+      </c>
+      <c r="N25" t="s">
         <v>654</v>
       </c>
-      <c r="N25" t="s">
-        <v>655</v>
-      </c>
       <c r="P25" t="s">
+        <v>705</v>
+      </c>
+      <c r="Q25" t="s">
         <v>706</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>440</v>
+      </c>
+      <c r="B26" t="s">
         <v>441</v>
       </c>
-      <c r="B26" t="s">
-        <v>442</v>
-      </c>
       <c r="D26" t="s">
+        <v>497</v>
+      </c>
+      <c r="E26" t="s">
         <v>498</v>
       </c>
-      <c r="E26" t="s">
-        <v>499</v>
-      </c>
       <c r="G26" t="s">
+        <v>549</v>
+      </c>
+      <c r="H26" t="s">
         <v>550</v>
       </c>
-      <c r="H26" t="s">
-        <v>551</v>
-      </c>
       <c r="J26" t="s">
+        <v>602</v>
+      </c>
+      <c r="K26" t="s">
         <v>603</v>
       </c>
-      <c r="K26" t="s">
-        <v>604</v>
-      </c>
       <c r="M26" t="s">
+        <v>655</v>
+      </c>
+      <c r="N26" t="s">
         <v>656</v>
       </c>
-      <c r="N26" t="s">
-        <v>657</v>
-      </c>
       <c r="P26" t="s">
+        <v>707</v>
+      </c>
+      <c r="Q26" t="s">
         <v>708</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>442</v>
+      </c>
+      <c r="B27" t="s">
         <v>443</v>
       </c>
-      <c r="B27" t="s">
-        <v>444</v>
-      </c>
       <c r="D27" t="s">
+        <v>499</v>
+      </c>
+      <c r="E27" t="s">
         <v>500</v>
       </c>
-      <c r="E27" t="s">
-        <v>501</v>
-      </c>
       <c r="G27" t="s">
+        <v>551</v>
+      </c>
+      <c r="H27" t="s">
         <v>552</v>
-      </c>
-      <c r="H27" t="s">
-        <v>553</v>
       </c>
       <c r="J27" t="s">
         <v>166</v>
       </c>
       <c r="K27" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="M27" t="s">
+        <v>657</v>
+      </c>
+      <c r="N27" t="s">
         <v>658</v>
       </c>
-      <c r="N27" t="s">
-        <v>659</v>
-      </c>
       <c r="P27" t="s">
+        <v>709</v>
+      </c>
+      <c r="Q27" t="s">
         <v>710</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>444</v>
+      </c>
+      <c r="B28" t="s">
         <v>445</v>
-      </c>
-      <c r="B28" t="s">
-        <v>446</v>
       </c>
       <c r="D28" t="s">
         <v>358</v>
       </c>
       <c r="E28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G28" t="s">
+        <v>553</v>
+      </c>
+      <c r="H28" t="s">
         <v>554</v>
       </c>
-      <c r="H28" t="s">
-        <v>555</v>
-      </c>
       <c r="J28" t="s">
+        <v>605</v>
+      </c>
+      <c r="K28" t="s">
         <v>606</v>
       </c>
-      <c r="K28" t="s">
-        <v>607</v>
-      </c>
       <c r="M28" t="s">
+        <v>659</v>
+      </c>
+      <c r="N28" t="s">
         <v>660</v>
-      </c>
-      <c r="N28" t="s">
-        <v>661</v>
       </c>
       <c r="P28" t="s">
         <v>298</v>
       </c>
       <c r="Q28" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -6236,51 +6236,51 @@
         <v>245</v>
       </c>
       <c r="B29" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D29" t="s">
+        <v>502</v>
+      </c>
+      <c r="E29" t="s">
         <v>503</v>
       </c>
-      <c r="E29" t="s">
-        <v>504</v>
-      </c>
       <c r="G29" t="s">
+        <v>555</v>
+      </c>
+      <c r="H29" t="s">
         <v>556</v>
       </c>
-      <c r="H29" t="s">
-        <v>557</v>
-      </c>
       <c r="J29" t="s">
+        <v>607</v>
+      </c>
+      <c r="K29" t="s">
         <v>608</v>
       </c>
-      <c r="K29" t="s">
-        <v>609</v>
-      </c>
       <c r="M29" t="s">
+        <v>661</v>
+      </c>
+      <c r="N29" t="s">
         <v>662</v>
       </c>
-      <c r="N29" t="s">
-        <v>663</v>
-      </c>
       <c r="P29" t="s">
+        <v>712</v>
+      </c>
+      <c r="Q29" t="s">
         <v>713</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>447</v>
+      </c>
+      <c r="B30" t="s">
         <v>448</v>
       </c>
-      <c r="B30" t="s">
-        <v>449</v>
-      </c>
       <c r="D30" t="s">
+        <v>504</v>
+      </c>
+      <c r="E30" t="s">
         <v>505</v>
-      </c>
-      <c r="E30" t="s">
-        <v>506</v>
       </c>
       <c r="G30" t="s">
         <v>42</v>
@@ -6289,22 +6289,22 @@
         <v>106</v>
       </c>
       <c r="J30" t="s">
+        <v>609</v>
+      </c>
+      <c r="K30" t="s">
         <v>610</v>
       </c>
-      <c r="K30" t="s">
-        <v>611</v>
-      </c>
       <c r="M30" t="s">
+        <v>663</v>
+      </c>
+      <c r="N30" t="s">
         <v>664</v>
       </c>
-      <c r="N30" t="s">
-        <v>665</v>
-      </c>
       <c r="P30" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q30" t="s">
         <v>715</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -6338,1262 +6338,1262 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B1" t="s">
         <v>748</v>
       </c>
-      <c r="B1" t="s">
-        <v>749</v>
-      </c>
       <c r="D1" t="s">
+        <v>806</v>
+      </c>
+      <c r="E1" t="s">
         <v>807</v>
       </c>
-      <c r="E1" t="s">
-        <v>808</v>
-      </c>
       <c r="G1" t="s">
+        <v>859</v>
+      </c>
+      <c r="H1" t="s">
         <v>860</v>
       </c>
-      <c r="H1" t="s">
-        <v>861</v>
-      </c>
       <c r="J1" t="s">
+        <v>913</v>
+      </c>
+      <c r="K1" t="s">
         <v>914</v>
       </c>
-      <c r="K1" t="s">
-        <v>915</v>
-      </c>
       <c r="M1" t="s">
+        <v>971</v>
+      </c>
+      <c r="N1" t="s">
         <v>972</v>
       </c>
-      <c r="N1" t="s">
-        <v>973</v>
-      </c>
       <c r="P1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="Q1" t="s">
         <v>1029</v>
       </c>
-      <c r="Q1" t="s">
-        <v>1030</v>
-      </c>
       <c r="S1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="T1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>749</v>
+      </c>
+      <c r="B2" t="s">
         <v>750</v>
       </c>
-      <c r="B2" t="s">
-        <v>751</v>
-      </c>
       <c r="D2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E2" t="s">
         <v>809</v>
       </c>
-      <c r="E2" t="s">
-        <v>810</v>
-      </c>
       <c r="G2" t="s">
+        <v>861</v>
+      </c>
+      <c r="H2" t="s">
         <v>862</v>
       </c>
-      <c r="H2" t="s">
-        <v>863</v>
-      </c>
       <c r="J2" t="s">
+        <v>915</v>
+      </c>
+      <c r="K2" t="s">
         <v>916</v>
       </c>
-      <c r="K2" t="s">
-        <v>917</v>
-      </c>
       <c r="M2" t="s">
+        <v>973</v>
+      </c>
+      <c r="N2" t="s">
         <v>974</v>
       </c>
-      <c r="N2" t="s">
-        <v>975</v>
-      </c>
       <c r="P2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="Q2" t="s">
         <v>1031</v>
       </c>
-      <c r="Q2" t="s">
-        <v>1032</v>
-      </c>
       <c r="S2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T2" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>751</v>
+      </c>
+      <c r="B3" t="s">
         <v>752</v>
       </c>
-      <c r="B3" t="s">
-        <v>753</v>
-      </c>
       <c r="D3" t="s">
+        <v>810</v>
+      </c>
+      <c r="E3" t="s">
         <v>811</v>
       </c>
-      <c r="E3" t="s">
-        <v>812</v>
-      </c>
       <c r="G3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J3" t="s">
+        <v>917</v>
+      </c>
+      <c r="K3" t="s">
         <v>918</v>
       </c>
-      <c r="K3" t="s">
-        <v>919</v>
-      </c>
       <c r="M3" t="s">
+        <v>975</v>
+      </c>
+      <c r="N3" t="s">
         <v>976</v>
       </c>
-      <c r="N3" t="s">
-        <v>977</v>
-      </c>
       <c r="P3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="Q3" t="s">
         <v>1033</v>
       </c>
-      <c r="Q3" t="s">
-        <v>1034</v>
-      </c>
       <c r="S3" t="s">
+        <v>1085</v>
+      </c>
+      <c r="T3" t="s">
         <v>1086</v>
-      </c>
-      <c r="T3" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>753</v>
+      </c>
+      <c r="B4" t="s">
         <v>754</v>
       </c>
-      <c r="B4" t="s">
-        <v>755</v>
-      </c>
       <c r="D4" t="s">
+        <v>812</v>
+      </c>
+      <c r="E4" t="s">
         <v>813</v>
       </c>
-      <c r="E4" t="s">
-        <v>814</v>
-      </c>
       <c r="G4" t="s">
+        <v>864</v>
+      </c>
+      <c r="H4" t="s">
         <v>865</v>
       </c>
-      <c r="H4" t="s">
-        <v>866</v>
-      </c>
       <c r="J4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="M4" t="s">
+        <v>977</v>
+      </c>
+      <c r="N4" t="s">
         <v>978</v>
       </c>
-      <c r="N4" t="s">
-        <v>979</v>
-      </c>
       <c r="P4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="Q4" t="s">
         <v>1035</v>
       </c>
-      <c r="Q4" t="s">
-        <v>1036</v>
-      </c>
       <c r="S4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="T4" t="s">
         <v>1088</v>
-      </c>
-      <c r="T4" t="s">
-        <v>1089</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>755</v>
+      </c>
+      <c r="B5" t="s">
         <v>756</v>
       </c>
-      <c r="B5" t="s">
-        <v>757</v>
-      </c>
       <c r="D5" t="s">
+        <v>814</v>
+      </c>
+      <c r="E5" t="s">
         <v>815</v>
       </c>
-      <c r="E5" t="s">
-        <v>816</v>
-      </c>
       <c r="G5" t="s">
+        <v>866</v>
+      </c>
+      <c r="H5" t="s">
         <v>867</v>
       </c>
-      <c r="H5" t="s">
-        <v>868</v>
-      </c>
       <c r="J5" t="s">
+        <v>920</v>
+      </c>
+      <c r="K5" t="s">
         <v>921</v>
       </c>
-      <c r="K5" t="s">
-        <v>922</v>
-      </c>
       <c r="M5" t="s">
+        <v>979</v>
+      </c>
+      <c r="N5" t="s">
         <v>980</v>
       </c>
-      <c r="N5" t="s">
-        <v>981</v>
-      </c>
       <c r="P5" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="Q5" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="S5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="T5" t="s">
         <v>1090</v>
-      </c>
-      <c r="T5" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>757</v>
+      </c>
+      <c r="B6" t="s">
         <v>758</v>
       </c>
-      <c r="B6" t="s">
-        <v>759</v>
-      </c>
       <c r="D6" t="s">
+        <v>816</v>
+      </c>
+      <c r="E6" t="s">
         <v>817</v>
       </c>
-      <c r="E6" t="s">
-        <v>818</v>
-      </c>
       <c r="G6" t="s">
+        <v>868</v>
+      </c>
+      <c r="H6" t="s">
         <v>869</v>
       </c>
-      <c r="H6" t="s">
-        <v>870</v>
-      </c>
       <c r="J6" t="s">
+        <v>922</v>
+      </c>
+      <c r="K6" t="s">
         <v>923</v>
       </c>
-      <c r="K6" t="s">
-        <v>924</v>
-      </c>
       <c r="M6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="N6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="Q6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="S6" t="s">
+        <v>1091</v>
+      </c>
+      <c r="T6" t="s">
         <v>1092</v>
-      </c>
-      <c r="T6" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>759</v>
+      </c>
+      <c r="B7" t="s">
         <v>760</v>
       </c>
-      <c r="B7" t="s">
-        <v>761</v>
-      </c>
       <c r="D7" t="s">
+        <v>818</v>
+      </c>
+      <c r="E7" t="s">
         <v>819</v>
       </c>
-      <c r="E7" t="s">
-        <v>820</v>
-      </c>
       <c r="G7" t="s">
+        <v>870</v>
+      </c>
+      <c r="H7" t="s">
         <v>871</v>
       </c>
-      <c r="H7" t="s">
-        <v>872</v>
-      </c>
       <c r="J7" t="s">
+        <v>924</v>
+      </c>
+      <c r="K7" t="s">
         <v>925</v>
       </c>
-      <c r="K7" t="s">
-        <v>926</v>
-      </c>
       <c r="M7" t="s">
+        <v>982</v>
+      </c>
+      <c r="N7" t="s">
         <v>983</v>
       </c>
-      <c r="N7" t="s">
-        <v>984</v>
-      </c>
       <c r="P7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Q7" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="S7" t="s">
+        <v>1093</v>
+      </c>
+      <c r="T7" t="s">
         <v>1094</v>
-      </c>
-      <c r="T7" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>761</v>
+      </c>
+      <c r="B8" t="s">
         <v>762</v>
       </c>
-      <c r="B8" t="s">
-        <v>763</v>
-      </c>
       <c r="D8" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="G8" t="s">
+        <v>872</v>
+      </c>
+      <c r="H8" t="s">
         <v>873</v>
       </c>
-      <c r="H8" t="s">
-        <v>874</v>
-      </c>
       <c r="J8" t="s">
+        <v>926</v>
+      </c>
+      <c r="K8" t="s">
         <v>927</v>
       </c>
-      <c r="K8" t="s">
-        <v>928</v>
-      </c>
       <c r="M8" t="s">
+        <v>984</v>
+      </c>
+      <c r="N8" t="s">
         <v>985</v>
       </c>
-      <c r="N8" t="s">
-        <v>986</v>
-      </c>
       <c r="P8" t="s">
+        <v>1039</v>
+      </c>
+      <c r="Q8" t="s">
         <v>1040</v>
       </c>
-      <c r="Q8" t="s">
-        <v>1041</v>
-      </c>
       <c r="S8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="T8" t="s">
         <v>1096</v>
-      </c>
-      <c r="T8" t="s">
-        <v>1097</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>763</v>
+      </c>
+      <c r="B9" t="s">
         <v>764</v>
       </c>
-      <c r="B9" t="s">
-        <v>765</v>
-      </c>
       <c r="D9" t="s">
+        <v>821</v>
+      </c>
+      <c r="E9" t="s">
         <v>822</v>
       </c>
-      <c r="E9" t="s">
-        <v>823</v>
-      </c>
       <c r="G9" t="s">
+        <v>874</v>
+      </c>
+      <c r="H9" t="s">
         <v>875</v>
       </c>
-      <c r="H9" t="s">
-        <v>876</v>
-      </c>
       <c r="J9" t="s">
+        <v>928</v>
+      </c>
+      <c r="K9" t="s">
         <v>929</v>
       </c>
-      <c r="K9" t="s">
-        <v>930</v>
-      </c>
       <c r="M9" t="s">
+        <v>986</v>
+      </c>
+      <c r="N9" t="s">
         <v>987</v>
       </c>
-      <c r="N9" t="s">
-        <v>988</v>
-      </c>
       <c r="P9" t="s">
+        <v>1041</v>
+      </c>
+      <c r="Q9" t="s">
         <v>1042</v>
       </c>
-      <c r="Q9" t="s">
-        <v>1043</v>
-      </c>
       <c r="S9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="T9" t="s">
         <v>1098</v>
-      </c>
-      <c r="T9" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>765</v>
+      </c>
+      <c r="B10" t="s">
         <v>766</v>
       </c>
-      <c r="B10" t="s">
-        <v>767</v>
-      </c>
       <c r="D10" t="s">
+        <v>823</v>
+      </c>
+      <c r="E10" t="s">
         <v>824</v>
       </c>
-      <c r="E10" t="s">
-        <v>825</v>
-      </c>
       <c r="G10" t="s">
+        <v>876</v>
+      </c>
+      <c r="H10" t="s">
         <v>877</v>
       </c>
-      <c r="H10" t="s">
-        <v>878</v>
-      </c>
       <c r="J10" t="s">
+        <v>930</v>
+      </c>
+      <c r="K10" t="s">
         <v>931</v>
       </c>
-      <c r="K10" t="s">
-        <v>932</v>
-      </c>
       <c r="M10" t="s">
+        <v>988</v>
+      </c>
+      <c r="N10" t="s">
         <v>989</v>
       </c>
-      <c r="N10" t="s">
-        <v>990</v>
-      </c>
       <c r="P10" t="s">
+        <v>1043</v>
+      </c>
+      <c r="Q10" t="s">
         <v>1044</v>
       </c>
-      <c r="Q10" t="s">
-        <v>1045</v>
-      </c>
       <c r="S10" t="s">
+        <v>1099</v>
+      </c>
+      <c r="T10" t="s">
         <v>1100</v>
-      </c>
-      <c r="T10" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>767</v>
+      </c>
+      <c r="B11" t="s">
         <v>768</v>
       </c>
-      <c r="B11" t="s">
-        <v>769</v>
-      </c>
       <c r="D11" t="s">
+        <v>825</v>
+      </c>
+      <c r="E11" t="s">
         <v>826</v>
       </c>
-      <c r="E11" t="s">
-        <v>827</v>
-      </c>
       <c r="G11" t="s">
+        <v>878</v>
+      </c>
+      <c r="H11" t="s">
         <v>879</v>
       </c>
-      <c r="H11" t="s">
-        <v>880</v>
-      </c>
       <c r="J11" t="s">
+        <v>932</v>
+      </c>
+      <c r="K11" t="s">
         <v>933</v>
       </c>
-      <c r="K11" t="s">
-        <v>934</v>
-      </c>
       <c r="M11" t="s">
+        <v>990</v>
+      </c>
+      <c r="N11" t="s">
         <v>991</v>
       </c>
-      <c r="N11" t="s">
-        <v>992</v>
-      </c>
       <c r="P11" t="s">
+        <v>1045</v>
+      </c>
+      <c r="Q11" t="s">
         <v>1046</v>
       </c>
-      <c r="Q11" t="s">
-        <v>1047</v>
-      </c>
       <c r="S11" t="s">
+        <v>1101</v>
+      </c>
+      <c r="T11" t="s">
         <v>1102</v>
-      </c>
-      <c r="T11" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>769</v>
+      </c>
+      <c r="B12" t="s">
         <v>770</v>
       </c>
-      <c r="B12" t="s">
-        <v>771</v>
-      </c>
       <c r="D12" t="s">
+        <v>827</v>
+      </c>
+      <c r="E12" t="s">
         <v>828</v>
       </c>
-      <c r="E12" t="s">
-        <v>829</v>
-      </c>
       <c r="G12" t="s">
+        <v>880</v>
+      </c>
+      <c r="H12" t="s">
         <v>881</v>
       </c>
-      <c r="H12" t="s">
-        <v>882</v>
-      </c>
       <c r="J12" t="s">
+        <v>934</v>
+      </c>
+      <c r="K12" t="s">
         <v>935</v>
       </c>
-      <c r="K12" t="s">
-        <v>936</v>
-      </c>
       <c r="M12" t="s">
+        <v>992</v>
+      </c>
+      <c r="N12" t="s">
         <v>993</v>
       </c>
-      <c r="N12" t="s">
-        <v>994</v>
-      </c>
       <c r="P12" t="s">
+        <v>1047</v>
+      </c>
+      <c r="Q12" t="s">
         <v>1048</v>
       </c>
-      <c r="Q12" t="s">
-        <v>1049</v>
-      </c>
       <c r="S12" t="s">
+        <v>1103</v>
+      </c>
+      <c r="T12" t="s">
         <v>1104</v>
-      </c>
-      <c r="T12" t="s">
-        <v>1105</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>771</v>
+      </c>
+      <c r="B13" t="s">
         <v>772</v>
       </c>
-      <c r="B13" t="s">
-        <v>773</v>
-      </c>
       <c r="D13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E13" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G13" t="s">
+        <v>882</v>
+      </c>
+      <c r="H13" t="s">
         <v>883</v>
       </c>
-      <c r="H13" t="s">
-        <v>884</v>
-      </c>
       <c r="J13" t="s">
+        <v>936</v>
+      </c>
+      <c r="K13" t="s">
         <v>937</v>
       </c>
-      <c r="K13" t="s">
-        <v>938</v>
-      </c>
       <c r="M13" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="N13" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P13" t="s">
+        <v>1049</v>
+      </c>
+      <c r="Q13" t="s">
         <v>1050</v>
       </c>
-      <c r="Q13" t="s">
-        <v>1051</v>
-      </c>
       <c r="S13" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="T13" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>773</v>
+      </c>
+      <c r="B14" t="s">
         <v>774</v>
       </c>
-      <c r="B14" t="s">
-        <v>775</v>
-      </c>
       <c r="D14" t="s">
+        <v>830</v>
+      </c>
+      <c r="E14" t="s">
         <v>831</v>
       </c>
-      <c r="E14" t="s">
-        <v>832</v>
-      </c>
       <c r="G14" t="s">
+        <v>884</v>
+      </c>
+      <c r="H14" t="s">
         <v>885</v>
       </c>
-      <c r="H14" t="s">
-        <v>886</v>
-      </c>
       <c r="J14" t="s">
+        <v>938</v>
+      </c>
+      <c r="K14" t="s">
         <v>939</v>
       </c>
-      <c r="K14" t="s">
-        <v>940</v>
-      </c>
       <c r="M14" t="s">
+        <v>995</v>
+      </c>
+      <c r="N14" t="s">
         <v>996</v>
       </c>
-      <c r="N14" t="s">
-        <v>997</v>
-      </c>
       <c r="P14" t="s">
+        <v>1051</v>
+      </c>
+      <c r="Q14" t="s">
         <v>1052</v>
       </c>
-      <c r="Q14" t="s">
-        <v>1053</v>
-      </c>
       <c r="S14" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T14" t="s">
         <v>1107</v>
-      </c>
-      <c r="T14" t="s">
-        <v>1108</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B15" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D15" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E15" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="G15" t="s">
+        <v>886</v>
+      </c>
+      <c r="H15" t="s">
         <v>887</v>
       </c>
-      <c r="H15" t="s">
-        <v>888</v>
-      </c>
       <c r="J15" t="s">
+        <v>940</v>
+      </c>
+      <c r="K15" t="s">
         <v>941</v>
       </c>
-      <c r="K15" t="s">
-        <v>942</v>
-      </c>
       <c r="M15" t="s">
+        <v>997</v>
+      </c>
+      <c r="N15" t="s">
         <v>998</v>
       </c>
-      <c r="N15" t="s">
-        <v>999</v>
-      </c>
       <c r="P15" t="s">
+        <v>1053</v>
+      </c>
+      <c r="Q15" t="s">
         <v>1054</v>
       </c>
-      <c r="Q15" t="s">
-        <v>1055</v>
-      </c>
       <c r="S15" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="T15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>776</v>
+      </c>
+      <c r="B16" t="s">
         <v>777</v>
       </c>
-      <c r="B16" t="s">
-        <v>778</v>
-      </c>
       <c r="D16" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G16" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J16" t="s">
+        <v>942</v>
+      </c>
+      <c r="K16" t="s">
         <v>943</v>
       </c>
-      <c r="K16" t="s">
-        <v>944</v>
-      </c>
       <c r="M16" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="N16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="P16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="Q16" t="s">
         <v>1056</v>
       </c>
-      <c r="Q16" t="s">
-        <v>1057</v>
-      </c>
       <c r="S16" t="s">
+        <v>1109</v>
+      </c>
+      <c r="T16" t="s">
         <v>1110</v>
-      </c>
-      <c r="T16" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>778</v>
+      </c>
+      <c r="B17" t="s">
         <v>779</v>
       </c>
-      <c r="B17" t="s">
-        <v>780</v>
-      </c>
       <c r="D17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E17" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G17" t="s">
+        <v>889</v>
+      </c>
+      <c r="H17" t="s">
         <v>890</v>
       </c>
-      <c r="H17" t="s">
-        <v>891</v>
-      </c>
       <c r="J17" t="s">
+        <v>944</v>
+      </c>
+      <c r="K17" t="s">
         <v>945</v>
       </c>
-      <c r="K17" t="s">
-        <v>946</v>
-      </c>
       <c r="M17" t="s">
+        <v>1000</v>
+      </c>
+      <c r="N17" t="s">
         <v>1001</v>
       </c>
-      <c r="N17" t="s">
-        <v>1002</v>
-      </c>
       <c r="P17" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Q17" t="s">
         <v>1058</v>
       </c>
-      <c r="Q17" t="s">
-        <v>1059</v>
-      </c>
       <c r="S17" t="s">
+        <v>1111</v>
+      </c>
+      <c r="T17" t="s">
         <v>1112</v>
-      </c>
-      <c r="T17" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>780</v>
+      </c>
+      <c r="B18" t="s">
         <v>781</v>
       </c>
-      <c r="B18" t="s">
-        <v>782</v>
-      </c>
       <c r="D18" t="s">
+        <v>836</v>
+      </c>
+      <c r="E18" t="s">
         <v>837</v>
       </c>
-      <c r="E18" t="s">
-        <v>838</v>
-      </c>
       <c r="G18" t="s">
+        <v>891</v>
+      </c>
+      <c r="H18" t="s">
         <v>892</v>
       </c>
-      <c r="H18" t="s">
-        <v>893</v>
-      </c>
       <c r="J18" t="s">
+        <v>946</v>
+      </c>
+      <c r="K18" t="s">
         <v>947</v>
       </c>
-      <c r="K18" t="s">
-        <v>948</v>
-      </c>
       <c r="M18" t="s">
+        <v>1002</v>
+      </c>
+      <c r="N18" t="s">
         <v>1003</v>
       </c>
-      <c r="N18" t="s">
-        <v>1004</v>
-      </c>
       <c r="P18" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Q18" t="s">
         <v>1060</v>
       </c>
-      <c r="Q18" t="s">
-        <v>1061</v>
-      </c>
       <c r="S18" t="s">
+        <v>1113</v>
+      </c>
+      <c r="T18" t="s">
         <v>1114</v>
-      </c>
-      <c r="T18" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>782</v>
+      </c>
+      <c r="B19" t="s">
         <v>783</v>
       </c>
-      <c r="B19" t="s">
-        <v>784</v>
-      </c>
       <c r="D19" t="s">
+        <v>838</v>
+      </c>
+      <c r="E19" t="s">
         <v>839</v>
       </c>
-      <c r="E19" t="s">
-        <v>840</v>
-      </c>
       <c r="G19" t="s">
+        <v>893</v>
+      </c>
+      <c r="H19" t="s">
         <v>894</v>
       </c>
-      <c r="H19" t="s">
-        <v>895</v>
-      </c>
       <c r="J19" t="s">
+        <v>948</v>
+      </c>
+      <c r="K19" t="s">
         <v>949</v>
       </c>
-      <c r="K19" t="s">
-        <v>950</v>
-      </c>
       <c r="M19" t="s">
+        <v>1004</v>
+      </c>
+      <c r="N19" t="s">
         <v>1005</v>
       </c>
-      <c r="N19" t="s">
-        <v>1006</v>
-      </c>
       <c r="P19" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Q19" t="s">
         <v>1062</v>
       </c>
-      <c r="Q19" t="s">
-        <v>1063</v>
-      </c>
       <c r="S19" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="T19" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>784</v>
+      </c>
+      <c r="B20" t="s">
         <v>785</v>
       </c>
-      <c r="B20" t="s">
-        <v>786</v>
-      </c>
       <c r="D20" t="s">
+        <v>840</v>
+      </c>
+      <c r="E20" t="s">
         <v>841</v>
       </c>
-      <c r="E20" t="s">
-        <v>842</v>
-      </c>
       <c r="G20" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H20" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J20" t="s">
+        <v>950</v>
+      </c>
+      <c r="K20" t="s">
         <v>951</v>
       </c>
-      <c r="K20" t="s">
-        <v>952</v>
-      </c>
       <c r="M20" t="s">
+        <v>1006</v>
+      </c>
+      <c r="N20" t="s">
         <v>1007</v>
       </c>
-      <c r="N20" t="s">
-        <v>1008</v>
-      </c>
       <c r="P20" t="s">
+        <v>1063</v>
+      </c>
+      <c r="Q20" t="s">
         <v>1064</v>
       </c>
-      <c r="Q20" t="s">
-        <v>1065</v>
-      </c>
       <c r="S20" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T20" t="s">
         <v>1117</v>
-      </c>
-      <c r="T20" t="s">
-        <v>1118</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>786</v>
+      </c>
+      <c r="B21" t="s">
         <v>787</v>
       </c>
-      <c r="B21" t="s">
-        <v>788</v>
-      </c>
       <c r="D21" t="s">
+        <v>842</v>
+      </c>
+      <c r="E21" t="s">
         <v>843</v>
       </c>
-      <c r="E21" t="s">
-        <v>844</v>
-      </c>
       <c r="G21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="J21" t="s">
+        <v>952</v>
+      </c>
+      <c r="K21" t="s">
         <v>953</v>
       </c>
-      <c r="K21" t="s">
-        <v>954</v>
-      </c>
       <c r="M21" t="s">
+        <v>1008</v>
+      </c>
+      <c r="N21" t="s">
         <v>1009</v>
       </c>
-      <c r="N21" t="s">
-        <v>1010</v>
-      </c>
       <c r="P21" t="s">
+        <v>1065</v>
+      </c>
+      <c r="Q21" t="s">
         <v>1066</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>788</v>
+      </c>
+      <c r="B22" t="s">
         <v>789</v>
       </c>
-      <c r="B22" t="s">
-        <v>790</v>
-      </c>
       <c r="D22" t="s">
+        <v>844</v>
+      </c>
+      <c r="E22" t="s">
         <v>845</v>
       </c>
-      <c r="E22" t="s">
-        <v>846</v>
-      </c>
       <c r="G22" t="s">
+        <v>897</v>
+      </c>
+      <c r="H22" t="s">
         <v>898</v>
       </c>
-      <c r="H22" t="s">
-        <v>899</v>
-      </c>
       <c r="J22" t="s">
+        <v>954</v>
+      </c>
+      <c r="K22" t="s">
         <v>955</v>
       </c>
-      <c r="K22" t="s">
-        <v>956</v>
-      </c>
       <c r="M22" t="s">
+        <v>1010</v>
+      </c>
+      <c r="N22" t="s">
         <v>1011</v>
       </c>
-      <c r="N22" t="s">
-        <v>1012</v>
-      </c>
       <c r="P22" t="s">
+        <v>1067</v>
+      </c>
+      <c r="Q22" t="s">
         <v>1068</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>790</v>
+      </c>
+      <c r="B23" t="s">
         <v>791</v>
       </c>
-      <c r="B23" t="s">
-        <v>792</v>
-      </c>
       <c r="D23" t="s">
+        <v>846</v>
+      </c>
+      <c r="E23" t="s">
         <v>847</v>
       </c>
-      <c r="E23" t="s">
-        <v>848</v>
-      </c>
       <c r="G23" t="s">
+        <v>899</v>
+      </c>
+      <c r="H23" t="s">
         <v>900</v>
       </c>
-      <c r="H23" t="s">
-        <v>901</v>
-      </c>
       <c r="J23" t="s">
+        <v>956</v>
+      </c>
+      <c r="K23" t="s">
         <v>957</v>
       </c>
-      <c r="K23" t="s">
-        <v>958</v>
-      </c>
       <c r="M23" t="s">
+        <v>1012</v>
+      </c>
+      <c r="N23" t="s">
         <v>1013</v>
       </c>
-      <c r="N23" t="s">
-        <v>1014</v>
-      </c>
       <c r="P23" t="s">
+        <v>1069</v>
+      </c>
+      <c r="Q23" t="s">
         <v>1070</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>1071</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>792</v>
+      </c>
+      <c r="B24" t="s">
         <v>793</v>
       </c>
-      <c r="B24" t="s">
-        <v>794</v>
-      </c>
       <c r="D24" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E24" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G24" t="s">
+        <v>901</v>
+      </c>
+      <c r="H24" t="s">
         <v>902</v>
       </c>
-      <c r="H24" t="s">
-        <v>903</v>
-      </c>
       <c r="J24" t="s">
+        <v>958</v>
+      </c>
+      <c r="K24" t="s">
         <v>959</v>
       </c>
-      <c r="K24" t="s">
-        <v>960</v>
-      </c>
       <c r="M24" t="s">
+        <v>1014</v>
+      </c>
+      <c r="N24" t="s">
         <v>1015</v>
       </c>
-      <c r="N24" t="s">
-        <v>1016</v>
-      </c>
       <c r="P24" t="s">
+        <v>1071</v>
+      </c>
+      <c r="Q24" t="s">
         <v>1072</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>1073</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>794</v>
+      </c>
+      <c r="B25" t="s">
         <v>795</v>
       </c>
-      <c r="B25" t="s">
-        <v>796</v>
-      </c>
       <c r="D25" t="s">
+        <v>849</v>
+      </c>
+      <c r="E25" t="s">
         <v>850</v>
       </c>
-      <c r="E25" t="s">
-        <v>851</v>
-      </c>
       <c r="G25" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="H25" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J25" t="s">
+        <v>960</v>
+      </c>
+      <c r="K25" t="s">
         <v>961</v>
       </c>
-      <c r="K25" t="s">
-        <v>962</v>
-      </c>
       <c r="M25" t="s">
+        <v>1016</v>
+      </c>
+      <c r="N25" t="s">
         <v>1017</v>
       </c>
-      <c r="N25" t="s">
-        <v>1018</v>
-      </c>
       <c r="P25" t="s">
+        <v>1073</v>
+      </c>
+      <c r="Q25" t="s">
         <v>1074</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>796</v>
+      </c>
+      <c r="B26" t="s">
         <v>797</v>
       </c>
-      <c r="B26" t="s">
-        <v>798</v>
-      </c>
       <c r="D26" t="s">
+        <v>851</v>
+      </c>
+      <c r="E26" t="s">
         <v>852</v>
       </c>
-      <c r="E26" t="s">
-        <v>853</v>
-      </c>
       <c r="G26" t="s">
+        <v>904</v>
+      </c>
+      <c r="H26" t="s">
         <v>905</v>
       </c>
-      <c r="H26" t="s">
-        <v>906</v>
-      </c>
       <c r="J26" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="K26" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M26" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N26" t="s">
         <v>1019</v>
       </c>
-      <c r="N26" t="s">
-        <v>1020</v>
-      </c>
       <c r="P26" t="s">
+        <v>1075</v>
+      </c>
+      <c r="Q26" t="s">
         <v>1076</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>798</v>
+      </c>
+      <c r="B27" t="s">
         <v>799</v>
       </c>
-      <c r="B27" t="s">
-        <v>800</v>
-      </c>
       <c r="D27" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E27" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G27" t="s">
+        <v>906</v>
+      </c>
+      <c r="H27" t="s">
         <v>907</v>
       </c>
-      <c r="H27" t="s">
-        <v>908</v>
-      </c>
       <c r="J27" t="s">
+        <v>963</v>
+      </c>
+      <c r="K27" t="s">
         <v>964</v>
       </c>
-      <c r="K27" t="s">
-        <v>965</v>
-      </c>
       <c r="M27" t="s">
+        <v>1020</v>
+      </c>
+      <c r="N27" t="s">
         <v>1021</v>
       </c>
-      <c r="N27" t="s">
-        <v>1022</v>
-      </c>
       <c r="P27" t="s">
+        <v>1077</v>
+      </c>
+      <c r="Q27" t="s">
         <v>1078</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>1079</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>800</v>
+      </c>
+      <c r="B28" t="s">
         <v>801</v>
       </c>
-      <c r="B28" t="s">
-        <v>802</v>
-      </c>
       <c r="D28" t="s">
+        <v>853</v>
+      </c>
+      <c r="E28" t="s">
         <v>854</v>
       </c>
-      <c r="E28" t="s">
-        <v>855</v>
-      </c>
       <c r="G28" t="s">
+        <v>908</v>
+      </c>
+      <c r="H28" t="s">
         <v>909</v>
       </c>
-      <c r="H28" t="s">
-        <v>910</v>
-      </c>
       <c r="J28" t="s">
+        <v>965</v>
+      </c>
+      <c r="K28" t="s">
         <v>966</v>
       </c>
-      <c r="K28" t="s">
-        <v>967</v>
-      </c>
       <c r="M28" t="s">
+        <v>1022</v>
+      </c>
+      <c r="N28" t="s">
         <v>1023</v>
       </c>
-      <c r="N28" t="s">
-        <v>1024</v>
-      </c>
       <c r="P28" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="Q28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>802</v>
+      </c>
+      <c r="B29" t="s">
         <v>803</v>
       </c>
-      <c r="B29" t="s">
-        <v>804</v>
-      </c>
       <c r="D29" t="s">
+        <v>855</v>
+      </c>
+      <c r="E29" t="s">
         <v>856</v>
       </c>
-      <c r="E29" t="s">
-        <v>857</v>
-      </c>
       <c r="G29" t="s">
+        <v>910</v>
+      </c>
+      <c r="H29" t="s">
         <v>911</v>
       </c>
-      <c r="H29" t="s">
-        <v>912</v>
-      </c>
       <c r="J29" t="s">
+        <v>967</v>
+      </c>
+      <c r="K29" t="s">
         <v>968</v>
       </c>
-      <c r="K29" t="s">
-        <v>969</v>
-      </c>
       <c r="M29" t="s">
+        <v>1024</v>
+      </c>
+      <c r="N29" t="s">
         <v>1025</v>
       </c>
-      <c r="N29" t="s">
-        <v>1026</v>
-      </c>
       <c r="P29" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Q29" t="s">
         <v>1081</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>1082</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>804</v>
+      </c>
+      <c r="B30" t="s">
         <v>805</v>
       </c>
-      <c r="B30" t="s">
-        <v>806</v>
-      </c>
       <c r="D30" t="s">
+        <v>857</v>
+      </c>
+      <c r="E30" t="s">
         <v>858</v>
       </c>
-      <c r="E30" t="s">
-        <v>859</v>
-      </c>
       <c r="G30" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="H30" t="s">
         <v>262</v>
       </c>
       <c r="J30" t="s">
+        <v>969</v>
+      </c>
+      <c r="K30" t="s">
         <v>970</v>
       </c>
-      <c r="K30" t="s">
-        <v>971</v>
-      </c>
       <c r="M30" t="s">
+        <v>1026</v>
+      </c>
+      <c r="N30" t="s">
         <v>1027</v>
       </c>
-      <c r="N30" t="s">
-        <v>1028</v>
-      </c>
       <c r="P30" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="Q30" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>